<commit_message>
solve inconsistency of statistical results
</commit_message>
<xml_diff>
--- a/3. Bears_and_Bugs.jar_Metrics/Bugs_jar_Complexity_51_Avg.xlsx
+++ b/3. Bears_and_Bugs.jar_Metrics/Bugs_jar_Complexity_51_Avg.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="261">
   <si>
     <t>Bugs.jar (analysis done Today 04:38 most recent)</t>
   </si>
@@ -1518,9 +1518,6 @@
     <t>42 projects</t>
   </si>
   <si>
-    <t>Multi-Chunk &amp; Multi-Line Common</t>
-  </si>
-  <si>
     <t>Two-Factor Common</t>
   </si>
   <si>
@@ -1528,6 +1525,9 @@
   </si>
   <si>
     <t>Multi-Chunk-High-Edits-Avg-Repaired</t>
+  </si>
+  <si>
+    <t>Chunks &amp; Lines Common</t>
   </si>
 </sst>
 </file>
@@ -2660,10 +2660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF238"/>
+  <dimension ref="A1:AF242"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I200" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S217" sqref="S217"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A183" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A185" sqref="A185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -4821,8 +4821,8 @@
       <c r="L61" s="6">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="M61" s="6" t="s">
-        <v>85</v>
+      <c r="M61" s="6">
+        <v>1241</v>
       </c>
       <c r="N61" s="6">
         <v>68.92</v>
@@ -8139,8 +8139,8 @@
       <c r="L112" s="8">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="M112" s="8" t="s">
-        <v>85</v>
+      <c r="M112" s="8">
+        <v>1241</v>
       </c>
       <c r="N112" s="8">
         <v>68.92</v>
@@ -12275,8 +12275,8 @@
       <c r="L163" s="8">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="M163" s="8" t="s">
-        <v>85</v>
+      <c r="M163" s="8">
+        <v>1241</v>
       </c>
       <c r="N163" s="8">
         <v>68.92</v>
@@ -13888,7 +13888,7 @@
       </c>
       <c r="N189" s="14">
         <f t="shared" si="13"/>
-        <v>18.572199999999999</v>
+        <v>42.541372549019584</v>
       </c>
       <c r="O189" s="14">
         <f t="shared" si="13"/>
@@ -13945,7 +13945,7 @@
       </c>
       <c r="N190" s="14">
         <f t="shared" si="14"/>
-        <v>18.509399999999996</v>
+        <v>42.479803921568603</v>
       </c>
       <c r="O190" s="14">
         <f t="shared" si="14"/>
@@ -14002,7 +14002,7 @@
       </c>
       <c r="N191" s="14">
         <f t="shared" si="15"/>
-        <v>18.572199999999999</v>
+        <v>42.541372549019584</v>
       </c>
       <c r="O191" s="14">
         <f t="shared" si="15"/>
@@ -14026,7 +14026,7 @@
     </row>
     <row r="194" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A194" s="26" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B194" s="27"/>
       <c r="C194" s="27"/>
@@ -14042,7 +14042,7 @@
       <c r="M194" s="27"/>
       <c r="N194" s="27"/>
       <c r="R194" s="35" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="S194" s="35"/>
       <c r="T194" s="35"/>
@@ -14213,55 +14213,55 @@
         <v>243</v>
       </c>
       <c r="T197" s="28" t="e">
-        <f>AVERAGEIFS(B$75:B$125, $U$126:$U$176, "YES")</f>
+        <f t="shared" ref="T197:AF197" si="17">AVERAGEIFS(B$75:B$125, $U$126:$U$176, "YES")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U197" s="28" t="e">
-        <f>AVERAGEIFS(C$75:C$125, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V197" s="28" t="e">
-        <f>AVERAGEIFS(D$75:D$125, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W197" s="28" t="e">
-        <f>AVERAGEIFS(E$75:E$125, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X197" s="28" t="e">
-        <f>AVERAGEIFS(F$75:F$125, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y197" s="28" t="e">
-        <f>AVERAGEIFS(G$75:G$125, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z197" s="28" t="e">
-        <f>AVERAGEIFS(H$75:H$125, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA197" s="28" t="e">
-        <f>AVERAGEIFS(I$75:I$125, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB197" s="28" t="e">
-        <f>AVERAGEIFS(J$75:J$125, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC197" s="28" t="e">
-        <f>AVERAGEIFS(K$75:K$125, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD197" s="28" t="e">
-        <f>AVERAGEIFS(L$75:L$125, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE197" s="28" t="e">
-        <f>AVERAGEIFS(M$75:M$125, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF197" s="28" t="e">
-        <f>AVERAGEIFS(N$75:N$125, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -14278,51 +14278,51 @@
         <v>4.2279999999999998</v>
       </c>
       <c r="D198" s="28">
-        <f t="shared" ref="D198:O198" si="17">AVERAGEIFS(C$126:C$176, $P$75:$P$125, "=1", $P$126:$P$176, "=1")</f>
+        <f t="shared" ref="D198:O198" si="18">AVERAGEIFS(C$126:C$176, $P$75:$P$125, "=1", $P$126:$P$176, "=1")</f>
         <v>75.234000000000009</v>
       </c>
       <c r="E198" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>30.006</v>
       </c>
       <c r="F198" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7.516</v>
       </c>
       <c r="G198" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>19.7</v>
       </c>
       <c r="H198" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>4.8609999999999998</v>
       </c>
       <c r="I198" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12.377000000000001</v>
       </c>
       <c r="J198" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>49.704999999999998</v>
       </c>
       <c r="K198" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>74.150999999999996</v>
       </c>
       <c r="L198" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.43</v>
       </c>
       <c r="M198" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>5.3200000000000004E-2</v>
       </c>
       <c r="N198" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7.6719999999999997</v>
       </c>
       <c r="O198" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.42599999999999999</v>
       </c>
       <c r="R198" s="1">
@@ -14333,55 +14333,55 @@
         <v>244</v>
       </c>
       <c r="T198" s="28" t="e">
-        <f>AVERAGEIFS(B$126:B$176, $U$126:$U$176, "YES")</f>
+        <f t="shared" ref="T198:AF198" si="19">AVERAGEIFS(B$126:B$176, $U$126:$U$176, "YES")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U198" s="28" t="e">
-        <f>AVERAGEIFS(C$126:C$176, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V198" s="28" t="e">
-        <f>AVERAGEIFS(D$126:D$176, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W198" s="28" t="e">
-        <f>AVERAGEIFS(E$126:E$176, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X198" s="28" t="e">
-        <f>AVERAGEIFS(F$126:F$176, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y198" s="28" t="e">
-        <f>AVERAGEIFS(G$126:G$176, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z198" s="28" t="e">
-        <f>AVERAGEIFS(H$126:H$176, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA198" s="28" t="e">
-        <f>AVERAGEIFS(I$126:I$176, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB198" s="28" t="e">
-        <f>AVERAGEIFS(J$126:J$176, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC198" s="28" t="e">
-        <f>AVERAGEIFS(K$126:K$176, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD198" s="28" t="e">
-        <f>AVERAGEIFS(L$126:L$176, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE198" s="28" t="e">
-        <f>AVERAGEIFS(M$126:M$176, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF198" s="28" t="e">
-        <f>AVERAGEIFS(N$126:N$176, $U$126:$U$176, "YES")</f>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -14487,51 +14487,51 @@
         <v>2.7747826086956535</v>
       </c>
       <c r="D201" s="28">
-        <f t="shared" ref="D201:O201" si="18">AVERAGEIFS(C$75:C$125, $P$75:$P$125, "&gt;1", $P$126:$P$176, "&gt;1")</f>
+        <f t="shared" ref="D201:O201" si="20">AVERAGEIFS(C$75:C$125, $P$75:$P$125, "&gt;1", $P$126:$P$176, "&gt;1")</f>
         <v>82.67434782608693</v>
       </c>
       <c r="E201" s="28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>16.830434782608698</v>
       </c>
       <c r="F201" s="28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>6.2204347826086979</v>
       </c>
       <c r="G201" s="28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>10.641739130434784</v>
       </c>
       <c r="H201" s="28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>3.5808695652173914</v>
       </c>
       <c r="I201" s="28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>9.800434782608697</v>
       </c>
       <c r="J201" s="28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>27.471304347826084</v>
       </c>
       <c r="K201" s="28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>50.61478260869567</v>
       </c>
       <c r="L201" s="28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.59034782608695657</v>
       </c>
       <c r="M201" s="28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>4.3217391304347832E-2</v>
       </c>
       <c r="N201" s="28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>24.85130434782609</v>
       </c>
       <c r="O201" s="28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>1.3800000000000003</v>
       </c>
       <c r="R201" s="1">
@@ -14542,55 +14542,55 @@
         <v>245</v>
       </c>
       <c r="T201" s="28">
-        <f>AVERAGEIFS(B$75:B$125, $V$126:$V$176, "YES")</f>
+        <f t="shared" ref="T201:AF201" si="21">AVERAGEIFS(B$75:B$125, $V$126:$V$176, "YES")</f>
         <v>4.0890000000000004</v>
       </c>
       <c r="U201" s="28">
-        <f>AVERAGEIFS(C$75:C$125, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="21"/>
         <v>75.169000000000011</v>
       </c>
       <c r="V201" s="28">
-        <f>AVERAGEIFS(D$75:D$125, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="21"/>
         <v>29.628999999999998</v>
       </c>
       <c r="W201" s="28">
-        <f>AVERAGEIFS(E$75:E$125, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="21"/>
         <v>7.5569999999999995</v>
       </c>
       <c r="X201" s="28">
-        <f>AVERAGEIFS(F$75:F$125, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="21"/>
         <v>19.756</v>
       </c>
       <c r="Y201" s="28">
-        <f>AVERAGEIFS(G$75:G$125, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="21"/>
         <v>4.8970000000000002</v>
       </c>
       <c r="Z201" s="28">
-        <f>AVERAGEIFS(H$75:H$125, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="21"/>
         <v>12.453999999999999</v>
       </c>
       <c r="AA201" s="28">
-        <f>AVERAGEIFS(I$75:I$125, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="21"/>
         <v>49.387999999999991</v>
       </c>
       <c r="AB201" s="28">
-        <f>AVERAGEIFS(J$75:J$125, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="21"/>
         <v>74.53</v>
       </c>
       <c r="AC201" s="28">
-        <f>AVERAGEIFS(K$75:K$125, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="21"/>
         <v>0.43</v>
       </c>
       <c r="AD201" s="28">
-        <f>AVERAGEIFS(L$75:L$125, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="21"/>
         <v>5.3200000000000004E-2</v>
       </c>
       <c r="AE201" s="28">
-        <f>AVERAGEIFS(M$75:M$125, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="21"/>
         <v>7.6719999999999997</v>
       </c>
       <c r="AF201" s="28">
-        <f>AVERAGEIFS(N$75:N$125, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="21"/>
         <v>0.42599999999999999</v>
       </c>
     </row>
@@ -14607,51 +14607,51 @@
         <v>2.6243478260869559</v>
       </c>
       <c r="D202" s="28">
-        <f t="shared" ref="D202:O202" si="19">AVERAGEIFS(C$126:C$176, $P$75:$P$125, "&gt;1", $P$126:$P$176, "&gt;1")</f>
+        <f t="shared" ref="D202:O202" si="22">AVERAGEIFS(C$126:C$176, $P$75:$P$125, "&gt;1", $P$126:$P$176, "&gt;1")</f>
         <v>82.895652173913035</v>
       </c>
       <c r="E202" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>16.311304347826088</v>
       </c>
       <c r="F202" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>6.253043478260869</v>
       </c>
       <c r="G202" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>10.121739130434781</v>
       </c>
       <c r="H202" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>3.463043478260869</v>
       </c>
       <c r="I202" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>9.715217391304348</v>
       </c>
       <c r="J202" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>26.432173913043474</v>
       </c>
       <c r="K202" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>49.544782608695662</v>
       </c>
       <c r="L202" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0.59739130434782606</v>
       </c>
       <c r="M202" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>4.3217391304347832E-2</v>
       </c>
       <c r="N202" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>24.987826086956527</v>
       </c>
       <c r="O202" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>1.3873913043478263</v>
       </c>
       <c r="R202" s="1">
@@ -14662,55 +14662,55 @@
         <v>246</v>
       </c>
       <c r="T202" s="28">
-        <f>AVERAGEIFS(B$126:B$176, $V$126:$V$176, "YES")</f>
+        <f t="shared" ref="T202:AF202" si="23">AVERAGEIFS(B$126:B$176, $V$126:$V$176, "YES")</f>
         <v>4.2279999999999998</v>
       </c>
       <c r="U202" s="28">
-        <f>AVERAGEIFS(C$126:C$176, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="23"/>
         <v>75.234000000000009</v>
       </c>
       <c r="V202" s="28">
-        <f>AVERAGEIFS(D$126:D$176, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="23"/>
         <v>30.006</v>
       </c>
       <c r="W202" s="28">
-        <f>AVERAGEIFS(E$126:E$176, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="23"/>
         <v>7.516</v>
       </c>
       <c r="X202" s="28">
-        <f>AVERAGEIFS(F$126:F$176, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="23"/>
         <v>19.7</v>
       </c>
       <c r="Y202" s="28">
-        <f>AVERAGEIFS(G$126:G$176, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="23"/>
         <v>4.8609999999999998</v>
       </c>
       <c r="Z202" s="28">
-        <f>AVERAGEIFS(H$126:H$176, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="23"/>
         <v>12.377000000000001</v>
       </c>
       <c r="AA202" s="28">
-        <f>AVERAGEIFS(I$126:I$176, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="23"/>
         <v>49.704999999999998</v>
       </c>
       <c r="AB202" s="28">
-        <f>AVERAGEIFS(J$126:J$176, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="23"/>
         <v>74.150999999999996</v>
       </c>
       <c r="AC202" s="28">
-        <f>AVERAGEIFS(K$126:K$176, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="23"/>
         <v>0.43</v>
       </c>
       <c r="AD202" s="28">
-        <f>AVERAGEIFS(L$126:L$176, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="23"/>
         <v>5.3200000000000004E-2</v>
       </c>
       <c r="AE202" s="28">
-        <f>AVERAGEIFS(M$126:M$176, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="23"/>
         <v>7.6719999999999997</v>
       </c>
       <c r="AF202" s="28">
-        <f>AVERAGEIFS(N$126:N$176, $V$126:$V$176, "YES")</f>
+        <f t="shared" si="23"/>
         <v>0.42599999999999999</v>
       </c>
     </row>
@@ -14842,51 +14842,51 @@
         <v>#DIV/0!</v>
       </c>
       <c r="D205" s="28" t="e">
-        <f t="shared" ref="D205:O205" si="20">AVERAGEIFS(C$75:C$125, $S$75:$S$125, "=1", $S$126:$S$176, "=1")</f>
+        <f t="shared" ref="D205:O205" si="24">AVERAGEIFS(C$75:C$125, $S$75:$S$125, "=1", $S$126:$S$176, "=1")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E205" s="28" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F205" s="28" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G205" s="28" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H205" s="28" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I205" s="28" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J205" s="28" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K205" s="28" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L205" s="28" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M205" s="28" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N205" s="28" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O205" s="28" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R205" s="1">
@@ -14897,55 +14897,55 @@
         <v>247</v>
       </c>
       <c r="T205" s="28" t="e">
-        <f>AVERAGEIFS(B$75:B$125, $W$126:$W$176, "YES")</f>
+        <f t="shared" ref="T205:AF205" si="25">AVERAGEIFS(B$75:B$125, $W$126:$W$176, "YES")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U205" s="28" t="e">
-        <f>AVERAGEIFS(C$75:C$125, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V205" s="28" t="e">
-        <f>AVERAGEIFS(D$75:D$125, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W205" s="28" t="e">
-        <f>AVERAGEIFS(E$75:E$125, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X205" s="28" t="e">
-        <f>AVERAGEIFS(F$75:F$125, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y205" s="28" t="e">
-        <f>AVERAGEIFS(G$75:G$125, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z205" s="28" t="e">
-        <f>AVERAGEIFS(H$75:H$125, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA205" s="28" t="e">
-        <f>AVERAGEIFS(I$75:I$125, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB205" s="28" t="e">
-        <f>AVERAGEIFS(J$75:J$125, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC205" s="28" t="e">
-        <f>AVERAGEIFS(K$75:K$125, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD205" s="28" t="e">
-        <f>AVERAGEIFS(L$75:L$125, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE205" s="28" t="e">
-        <f>AVERAGEIFS(M$75:M$125, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF205" s="28" t="e">
-        <f>AVERAGEIFS(N$75:N$125, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -14962,51 +14962,51 @@
         <v>#DIV/0!</v>
       </c>
       <c r="D206" s="28" t="e">
-        <f t="shared" ref="D206:O206" si="21">AVERAGEIFS(C$126:C$176, $S$75:$S$125, "=1", $S$126:$S$176, "=1")</f>
+        <f t="shared" ref="D206:O206" si="26">AVERAGEIFS(C$126:C$176, $S$75:$S$125, "=1", $S$126:$S$176, "=1")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E206" s="28" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F206" s="28" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G206" s="28" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H206" s="28" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I206" s="28" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J206" s="28" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K206" s="28" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L206" s="28" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M206" s="28" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N206" s="28" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O206" s="28" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R206" s="1">
@@ -15017,55 +15017,55 @@
         <v>248</v>
       </c>
       <c r="T206" s="28" t="e">
-        <f>AVERAGEIFS(B$126:B$176, $W$126:$W$176, "YES")</f>
+        <f t="shared" ref="T206:AF206" si="27">AVERAGEIFS(B$126:B$176, $W$126:$W$176, "YES")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U206" s="28" t="e">
-        <f>AVERAGEIFS(C$126:C$176, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V206" s="28" t="e">
-        <f>AVERAGEIFS(D$126:D$176, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W206" s="28" t="e">
-        <f>AVERAGEIFS(E$126:E$176, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X206" s="28" t="e">
-        <f>AVERAGEIFS(F$126:F$176, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y206" s="28" t="e">
-        <f>AVERAGEIFS(G$126:G$176, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z206" s="28" t="e">
-        <f>AVERAGEIFS(H$126:H$176, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA206" s="28" t="e">
-        <f>AVERAGEIFS(I$126:I$176, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB206" s="28" t="e">
-        <f>AVERAGEIFS(J$126:J$176, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC206" s="28" t="e">
-        <f>AVERAGEIFS(K$126:K$176, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD206" s="28" t="e">
-        <f>AVERAGEIFS(L$126:L$176, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE206" s="28" t="e">
-        <f>AVERAGEIFS(M$126:M$176, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF206" s="28" t="e">
-        <f>AVERAGEIFS(N$126:N$176, $W$126:$W$176, "YES")</f>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -15197,51 +15197,51 @@
         <v>3.4094117647058821</v>
       </c>
       <c r="D209" s="28">
-        <f t="shared" ref="D209:O209" si="22">AVERAGEIFS(C$75:C$125, $S$75:$S$125, "&gt;1", $S$126:$S$176, "&gt;1")</f>
+        <f t="shared" ref="D209:O209" si="28">AVERAGEIFS(C$75:C$125, $S$75:$S$125, "&gt;1", $S$126:$S$176, "&gt;1")</f>
         <v>78.530196078431388</v>
       </c>
       <c r="E209" s="28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>23.924901960784307</v>
       </c>
       <c r="F209" s="28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>7.3060784313725522</v>
       </c>
       <c r="G209" s="28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>15.764509803921564</v>
       </c>
       <c r="H209" s="28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>4.3756862745098033</v>
       </c>
       <c r="I209" s="28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>11.681372549019608</v>
       </c>
       <c r="J209" s="28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>39.690392156862735</v>
       </c>
       <c r="K209" s="28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>65.971568627450978</v>
       </c>
       <c r="L209" s="28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>0.55860784313725487</v>
       </c>
       <c r="M209" s="28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>4.592156862745099E-2</v>
       </c>
       <c r="N209" s="28">
-        <f t="shared" si="22"/>
-        <v>18.509399999999996</v>
+        <f t="shared" si="28"/>
+        <v>42.479803921568603</v>
       </c>
       <c r="O209" s="28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>2.3590392156862743</v>
       </c>
       <c r="R209" s="1">
@@ -15252,55 +15252,55 @@
         <v>249</v>
       </c>
       <c r="T209" s="28">
-        <f>AVERAGEIFS(B$75:B$125, $X$126:$X$176, "YES")</f>
+        <f t="shared" ref="T209:AF209" si="29">AVERAGEIFS(B$75:B$125, $X$126:$X$176, "YES")</f>
         <v>2.7845454545454555</v>
       </c>
       <c r="U209" s="28">
-        <f>AVERAGEIFS(C$75:C$125, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="29"/>
         <v>82.677272727272694</v>
       </c>
       <c r="V209" s="28">
-        <f>AVERAGEIFS(D$75:D$125, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="29"/>
         <v>17.105454545454545</v>
       </c>
       <c r="W209" s="28">
-        <f>AVERAGEIFS(E$75:E$125, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="29"/>
         <v>6.2481818181818198</v>
       </c>
       <c r="X209" s="28">
-        <f>AVERAGEIFS(F$75:F$125, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="29"/>
         <v>10.74909090909091</v>
       </c>
       <c r="Y209" s="28">
-        <f>AVERAGEIFS(G$75:G$125, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="29"/>
         <v>3.5818181818181816</v>
       </c>
       <c r="Z209" s="28">
-        <f>AVERAGEIFS(H$75:H$125, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="29"/>
         <v>9.82909090909091</v>
       </c>
       <c r="AA209" s="28">
-        <f>AVERAGEIFS(I$75:I$125, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="29"/>
         <v>27.853636363636358</v>
       </c>
       <c r="AB209" s="28">
-        <f>AVERAGEIFS(J$75:J$125, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="29"/>
         <v>50.912272727272736</v>
       </c>
       <c r="AC209" s="28">
-        <f>AVERAGEIFS(K$75:K$125, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="29"/>
         <v>0.59945454545454546</v>
       </c>
       <c r="AD209" s="28">
-        <f>AVERAGEIFS(L$75:L$125, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="29"/>
         <v>4.3409090909090925E-2</v>
       </c>
       <c r="AE209" s="28">
-        <f>AVERAGEIFS(M$75:M$125, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="29"/>
         <v>25.310909090909092</v>
       </c>
       <c r="AF209" s="28">
-        <f>AVERAGEIFS(N$75:N$125, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="29"/>
         <v>1.4054545454545457</v>
       </c>
     </row>
@@ -15317,51 +15317,51 @@
         <v>3.424509803921568</v>
       </c>
       <c r="D210" s="28">
-        <f t="shared" ref="D210:O210" si="23">AVERAGEIFS(C$126:C$176, $S$75:$S$125, "&gt;1", $S$126:$S$176, "&gt;1")</f>
+        <f t="shared" ref="D210:O210" si="30">AVERAGEIFS(C$126:C$176, $S$75:$S$125, "&gt;1", $S$126:$S$176, "&gt;1")</f>
         <v>78.645686274509828</v>
       </c>
       <c r="E210" s="28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>24.032549019607846</v>
       </c>
       <c r="F210" s="28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>7.3231372549019627</v>
       </c>
       <c r="G210" s="28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>15.519411764705881</v>
       </c>
       <c r="H210" s="28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>4.3221568627450981</v>
       </c>
       <c r="I210" s="28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>11.644705882352941</v>
       </c>
       <c r="J210" s="28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>39.550980392156859</v>
       </c>
       <c r="K210" s="28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>65.592745098039202</v>
       </c>
       <c r="L210" s="28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>0.56178431372549031</v>
       </c>
       <c r="M210" s="28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>4.592156862745099E-2</v>
       </c>
       <c r="N210" s="28">
-        <f t="shared" si="23"/>
-        <v>18.572199999999999</v>
+        <f t="shared" si="30"/>
+        <v>42.541372549019584</v>
       </c>
       <c r="O210" s="28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>2.3623725490196072</v>
       </c>
       <c r="R210" s="1">
@@ -15372,1402 +15372,1406 @@
         <v>250</v>
       </c>
       <c r="T210" s="28">
-        <f>AVERAGEIFS(B$126:B$176, $X$126:$X$176, "YES")</f>
+        <f t="shared" ref="T210:AF210" si="31">AVERAGEIFS(B$126:B$176, $X$126:$X$176, "YES")</f>
         <v>2.6377272727272723</v>
       </c>
       <c r="U210" s="28">
-        <f>AVERAGEIFS(C$126:C$176, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="31"/>
         <v>82.888181818181806</v>
       </c>
       <c r="V210" s="28">
-        <f>AVERAGEIFS(D$126:D$176, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="31"/>
         <v>16.61090909090909</v>
       </c>
       <c r="W210" s="28">
-        <f>AVERAGEIFS(E$126:E$176, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="31"/>
         <v>6.2845454545454542</v>
       </c>
       <c r="X210" s="28">
-        <f>AVERAGEIFS(F$126:F$176, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="31"/>
         <v>10.243636363636362</v>
       </c>
       <c r="Y210" s="28">
-        <f>AVERAGEIFS(G$126:G$176, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="31"/>
         <v>3.4663636363636368</v>
       </c>
       <c r="Z210" s="28">
-        <f>AVERAGEIFS(H$126:H$176, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="31"/>
         <v>9.750454545454545</v>
       </c>
       <c r="AA210" s="28">
-        <f>AVERAGEIFS(I$126:I$176, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="31"/>
         <v>26.853181818181817</v>
       </c>
       <c r="AB210" s="28">
-        <f>AVERAGEIFS(J$126:J$176, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="31"/>
         <v>49.9</v>
       </c>
       <c r="AC210" s="28">
-        <f>AVERAGEIFS(K$126:K$176, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="31"/>
         <v>0.60681818181818181</v>
       </c>
       <c r="AD210" s="28">
-        <f>AVERAGEIFS(L$126:L$176, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="31"/>
         <v>4.3409090909090925E-2</v>
       </c>
       <c r="AE210" s="28">
-        <f>AVERAGEIFS(M$126:M$176, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="31"/>
         <v>25.45363636363637</v>
       </c>
       <c r="AF210" s="28">
-        <f>AVERAGEIFS(N$126:N$176, $X$126:$X$176, "YES")</f>
+        <f t="shared" si="31"/>
         <v>1.4131818181818183</v>
       </c>
     </row>
-    <row r="212" spans="1:32" ht="43.2" x14ac:dyDescent="0.35">
-      <c r="R212" s="34"/>
-      <c r="S212" s="12" t="s">
+    <row r="212" spans="1:32" ht="28.8" x14ac:dyDescent="0.35">
+      <c r="A212" s="34"/>
+      <c r="B212" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="T212" s="12" t="s">
+      <c r="C212" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="U212" s="12" t="s">
+      <c r="D212" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="V212" s="12" t="s">
+      <c r="E212" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="W212" s="12" t="s">
+      <c r="F212" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="X212" s="12" t="s">
+      <c r="G212" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="Y212" s="12" t="s">
+      <c r="H212" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="Z212" s="12" t="s">
+      <c r="I212" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="AA212" s="12" t="s">
+      <c r="J212" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="AB212" s="12" t="s">
+      <c r="K212" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="AC212" s="12" t="s">
+      <c r="L212" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="AD212" s="12" t="s">
+      <c r="M212" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="AE212" s="12" t="s">
+      <c r="N212" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="AF212" s="12" t="s">
+      <c r="O212" s="12" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="213" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A213" s="26" t="s">
-        <v>215</v>
-      </c>
-      <c r="B213" s="27"/>
-      <c r="C213" s="27"/>
-      <c r="D213" s="27"/>
-      <c r="E213" s="27"/>
-      <c r="F213" s="27"/>
-      <c r="G213" s="27"/>
-      <c r="H213" s="27"/>
-      <c r="I213" s="27"/>
-      <c r="J213" s="27"/>
-      <c r="K213" s="27"/>
-      <c r="L213" s="27"/>
-      <c r="M213" s="27"/>
-      <c r="N213" s="27"/>
-      <c r="R213" s="1">
+      <c r="A213" s="1">
         <f>COUNTIFS($Y$126:$Y$176, "YES")</f>
         <v>26</v>
       </c>
-      <c r="S213" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="T213" s="28">
-        <f>AVERAGEIFS(B$75:B$125, $Y$126:$Y$176, "YES")</f>
+      <c r="B213" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C213" s="28">
+        <f t="shared" ref="C213:O213" si="32">AVERAGEIFS(B$75:B$125, $Y$126:$Y$176, "YES")</f>
         <v>3.8342307692307696</v>
       </c>
-      <c r="U213" s="28">
-        <f>AVERAGEIFS(C$75:C$125, $Y$126:$Y$176, "YES")</f>
+      <c r="D213" s="28">
+        <f t="shared" si="32"/>
         <v>75.066538461538443</v>
       </c>
-      <c r="V213" s="28">
-        <f>AVERAGEIFS(D$75:D$125, $Y$126:$Y$176, "YES")</f>
+      <c r="E213" s="28">
+        <f t="shared" si="32"/>
         <v>31.476153846153842</v>
       </c>
-      <c r="W213" s="28">
-        <f>AVERAGEIFS(E$75:E$125, $Y$126:$Y$176, "YES")</f>
+      <c r="F213" s="28">
+        <f t="shared" si="32"/>
         <v>8.7419230769230758</v>
       </c>
-      <c r="X213" s="28">
-        <f>AVERAGEIFS(F$75:F$125, $Y$126:$Y$176, "YES")</f>
+      <c r="G213" s="28">
+        <f t="shared" si="32"/>
         <v>20.19499999999999</v>
       </c>
-      <c r="Y213" s="28">
-        <f>AVERAGEIFS(G$75:G$125, $Y$126:$Y$176, "YES")</f>
+      <c r="H213" s="28">
+        <f t="shared" si="32"/>
         <v>4.8926923076923066</v>
       </c>
-      <c r="Z213" s="28">
-        <f>AVERAGEIFS(H$75:H$125, $Y$126:$Y$176, "YES")</f>
+      <c r="I213" s="28">
+        <f t="shared" si="32"/>
         <v>13.634615384615385</v>
       </c>
-      <c r="AA213" s="28">
-        <f>AVERAGEIFS(I$75:I$125, $Y$126:$Y$176, "YES")</f>
+      <c r="J213" s="28">
+        <f t="shared" si="32"/>
         <v>51.671538461538447</v>
       </c>
-      <c r="AB213" s="28">
-        <f>AVERAGEIFS(J$75:J$125, $Y$126:$Y$176, "YES")</f>
+      <c r="K213" s="28">
+        <f t="shared" si="32"/>
         <v>80.881153846153836</v>
       </c>
-      <c r="AC213" s="28">
-        <f>AVERAGEIFS(K$75:K$125, $Y$126:$Y$176, "YES")</f>
+      <c r="L213" s="28">
+        <f t="shared" si="32"/>
         <v>0.52419230769230762</v>
       </c>
-      <c r="AD213" s="28">
-        <f>AVERAGEIFS(L$75:L$125, $Y$126:$Y$176, "YES")</f>
+      <c r="M213" s="28">
+        <f t="shared" si="32"/>
         <v>4.1346153846153859E-2</v>
       </c>
-      <c r="AE213" s="28">
-        <f>AVERAGEIFS(M$75:M$125, $Y$126:$Y$176, "YES")</f>
+      <c r="N213" s="28">
+        <f t="shared" si="32"/>
         <v>21.885384615384616</v>
       </c>
-      <c r="AF213" s="28">
-        <f>AVERAGEIFS(N$75:N$125, $Y$126:$Y$176, "YES")</f>
+      <c r="O213" s="28">
+        <f t="shared" si="32"/>
         <v>1.2150384615384617</v>
       </c>
     </row>
-    <row r="214" spans="1:32" ht="15" x14ac:dyDescent="0.35">
-      <c r="A214"/>
-      <c r="B214"/>
-      <c r="C214"/>
-      <c r="D214"/>
-      <c r="E214"/>
-      <c r="F214"/>
-      <c r="G214"/>
-      <c r="H214"/>
-      <c r="I214"/>
-      <c r="J214"/>
-      <c r="K214"/>
-      <c r="L214"/>
-      <c r="M214"/>
-      <c r="N214"/>
-      <c r="R214" s="1">
+    <row r="214" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A214" s="1">
         <f>COUNTIFS($Y$126:$Y$176, "YES")</f>
         <v>26</v>
       </c>
-      <c r="S214" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="T214" s="28">
-        <f>AVERAGEIFS(B$126:B$176, $Y$126:$Y$176, "YES")</f>
+      <c r="B214" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C214" s="28">
+        <f t="shared" ref="C214:O214" si="33">AVERAGEIFS(B$126:B$176, $Y$126:$Y$176, "YES")</f>
         <v>3.9238461538461555</v>
       </c>
-      <c r="U214" s="28">
-        <f>AVERAGEIFS(C$126:C$176, $Y$126:$Y$176, "YES")</f>
+      <c r="D214" s="28">
+        <f t="shared" si="33"/>
         <v>75.171153846153828</v>
       </c>
-      <c r="V214" s="28">
-        <f>AVERAGEIFS(D$126:D$176, $Y$126:$Y$176, "YES")</f>
+      <c r="E214" s="28">
+        <f t="shared" si="33"/>
         <v>31.912307692307692</v>
       </c>
-      <c r="W214" s="28">
-        <f>AVERAGEIFS(E$126:E$176, $Y$126:$Y$176, "YES")</f>
+      <c r="F214" s="28">
+        <f t="shared" si="33"/>
         <v>8.7803846153846159</v>
       </c>
-      <c r="X214" s="28">
-        <f>AVERAGEIFS(F$126:F$176, $Y$126:$Y$176, "YES")</f>
+      <c r="G214" s="28">
+        <f t="shared" si="33"/>
         <v>19.922692307692312</v>
       </c>
-      <c r="Y214" s="28">
-        <f>AVERAGEIFS(G$126:G$176, $Y$126:$Y$176, "YES")</f>
+      <c r="H214" s="28">
+        <f t="shared" si="33"/>
         <v>4.8623076923076916</v>
       </c>
-      <c r="Z214" s="28">
-        <f>AVERAGEIFS(H$126:H$176, $Y$126:$Y$176, "YES")</f>
+      <c r="I214" s="28">
+        <f t="shared" si="33"/>
         <v>13.643076923076926</v>
       </c>
-      <c r="AA214" s="28">
-        <f>AVERAGEIFS(I$126:I$176, $Y$126:$Y$176, "YES")</f>
+      <c r="J214" s="28">
+        <f t="shared" si="33"/>
         <v>51.832307692307708</v>
       </c>
-      <c r="AB214" s="28">
-        <f>AVERAGEIFS(J$126:J$176, $Y$126:$Y$176, "YES")</f>
+      <c r="K214" s="28">
+        <f t="shared" si="33"/>
         <v>80.86615384615385</v>
       </c>
-      <c r="AC214" s="28">
-        <f>AVERAGEIFS(K$126:K$176, $Y$126:$Y$176, "YES")</f>
+      <c r="L214" s="28">
+        <f t="shared" si="33"/>
         <v>0.53042307692307678</v>
       </c>
-      <c r="AD214" s="28">
-        <f>AVERAGEIFS(L$126:L$176, $Y$126:$Y$176, "YES")</f>
+      <c r="M214" s="28">
+        <f t="shared" si="33"/>
         <v>4.1346153846153859E-2</v>
       </c>
-      <c r="AE214" s="28">
-        <f>AVERAGEIFS(M$126:M$176, $Y$126:$Y$176, "YES")</f>
+      <c r="N214" s="28">
+        <f t="shared" si="33"/>
         <v>22.006153846153843</v>
       </c>
-      <c r="AF214" s="28">
-        <f>AVERAGEIFS(N$126:N$176, $Y$126:$Y$176, "YES")</f>
+      <c r="O214" s="28">
+        <f t="shared" si="33"/>
         <v>1.2215769230769231</v>
       </c>
     </row>
-    <row r="215" spans="1:32" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A215" s="12" t="s">
+    <row r="217" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A217" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B217" s="27"/>
+      <c r="C217" s="27"/>
+      <c r="D217" s="27"/>
+      <c r="E217" s="27"/>
+      <c r="F217" s="27"/>
+      <c r="G217" s="27"/>
+      <c r="H217" s="27"/>
+      <c r="I217" s="27"/>
+      <c r="J217" s="27"/>
+      <c r="K217" s="27"/>
+      <c r="L217" s="27"/>
+      <c r="M217" s="27"/>
+      <c r="N217" s="27"/>
+    </row>
+    <row r="218" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+      <c r="A218"/>
+      <c r="B218"/>
+      <c r="C218"/>
+      <c r="D218"/>
+      <c r="E218"/>
+      <c r="F218"/>
+      <c r="G218"/>
+      <c r="H218"/>
+      <c r="I218"/>
+      <c r="J218"/>
+      <c r="K218"/>
+      <c r="L218"/>
+      <c r="M218"/>
+      <c r="N218"/>
+    </row>
+    <row r="219" spans="1:32" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A219" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="B215" s="12" t="s">
+      <c r="B219" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="C215" s="12" t="s">
+      <c r="C219" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="D215" s="12" t="s">
+      <c r="D219" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="E215" s="12" t="s">
+      <c r="E219" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="F215" s="12" t="s">
+      <c r="F219" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G215" s="12" t="s">
+      <c r="G219" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="H215" s="12" t="s">
+      <c r="H219" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I215" s="12" t="s">
+      <c r="I219" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="J215" s="12" t="s">
+      <c r="J219" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="K215" s="12" t="s">
+      <c r="K219" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="L215" s="12" t="s">
+      <c r="L219" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="M215" s="12" t="s">
+      <c r="M219" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="N215" s="12" t="s">
+      <c r="N219" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="O215" s="12" t="s">
+      <c r="O219" s="12" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="216" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A216" s="1">
+    <row r="220" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A220" s="1">
         <f>COUNTIF($A$24:$A$176, "*Commons-Math*Buggy")</f>
         <v>49</v>
       </c>
-      <c r="B216" s="1" t="s">
+      <c r="B220" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C216" s="28">
-        <f t="shared" ref="C216:O216" si="24">AVERAGEIF($A$24:$A$176, "*Commons-Math*_Buggy", B$24:B$176)</f>
+      <c r="C220" s="28">
+        <f t="shared" ref="C220:O220" si="34">AVERAGEIF($A$24:$A$176, "*Commons-Math*_Buggy", B$24:B$176)</f>
         <v>3.2914285714285727</v>
       </c>
-      <c r="D216" s="28">
-        <f t="shared" si="24"/>
+      <c r="D220" s="28">
+        <f t="shared" si="34"/>
         <v>78.420204081632633</v>
       </c>
-      <c r="E216" s="28">
-        <f t="shared" si="24"/>
+      <c r="E220" s="28">
+        <f t="shared" si="34"/>
         <v>24.387551020408157</v>
       </c>
-      <c r="F216" s="28">
-        <f t="shared" si="24"/>
+      <c r="F220" s="28">
+        <f t="shared" si="34"/>
         <v>7.4553061224489783</v>
       </c>
-      <c r="G216" s="28">
-        <f t="shared" si="24"/>
+      <c r="G220" s="28">
+        <f t="shared" si="34"/>
         <v>15.391020408163268</v>
       </c>
-      <c r="H216" s="28">
-        <f t="shared" si="24"/>
+      <c r="H220" s="28">
+        <f t="shared" si="34"/>
         <v>4.3769387755102036</v>
       </c>
-      <c r="I216" s="28">
-        <f t="shared" si="24"/>
+      <c r="I220" s="28">
+        <f t="shared" si="34"/>
         <v>11.832857142857142</v>
       </c>
-      <c r="J216" s="28">
-        <f t="shared" si="24"/>
+      <c r="J220" s="28">
+        <f t="shared" si="34"/>
         <v>39.778979591836716</v>
       </c>
-      <c r="K216" s="28">
-        <f t="shared" si="24"/>
+      <c r="K220" s="28">
+        <f t="shared" si="34"/>
         <v>66.847959183673467</v>
       </c>
-      <c r="L216" s="28">
-        <f t="shared" si="24"/>
+      <c r="L220" s="28">
+        <f t="shared" si="34"/>
         <v>0.58471428571428574</v>
       </c>
-      <c r="M216" s="28">
-        <f t="shared" si="24"/>
+      <c r="M220" s="28">
+        <f t="shared" si="34"/>
         <v>4.7795918367346951E-2</v>
       </c>
-      <c r="N216" s="28">
-        <f t="shared" si="24"/>
-        <v>19.346041666666665</v>
-      </c>
-      <c r="O216" s="28">
-        <f t="shared" si="24"/>
+      <c r="N220" s="28">
+        <f t="shared" si="34"/>
+        <v>44.277755102040793</v>
+      </c>
+      <c r="O220" s="28">
+        <f t="shared" si="34"/>
         <v>2.4587959183673465</v>
       </c>
     </row>
-    <row r="217" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A217" s="1">
+    <row r="221" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A221" s="1">
         <f>COUNTIF($A$24:$A$176, "*Commons-Math*Fixed")</f>
         <v>49</v>
       </c>
-      <c r="B217" s="1" t="s">
+      <c r="B221" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C217" s="28">
-        <f t="shared" ref="C217:O217" si="25">AVERAGEIF($A$24:$A$176, "*Commons-Math*_Fixed", B$24:B$176)</f>
+      <c r="C221" s="28">
+        <f t="shared" ref="C221:O221" si="35">AVERAGEIF($A$24:$A$176, "*Commons-Math*_Fixed", B$24:B$176)</f>
         <v>3.4824489795918359</v>
       </c>
-      <c r="D217" s="28">
-        <f t="shared" si="25"/>
+      <c r="D221" s="28">
+        <f t="shared" si="35"/>
         <v>78.184489795918381</v>
       </c>
-      <c r="E217" s="28">
-        <f t="shared" si="25"/>
+      <c r="E221" s="28">
+        <f t="shared" si="35"/>
         <v>24.610816326530603</v>
       </c>
-      <c r="F217" s="28">
-        <f t="shared" si="25"/>
+      <c r="F221" s="28">
+        <f t="shared" si="35"/>
         <v>7.4614285714285753</v>
       </c>
-      <c r="G217" s="28">
-        <f t="shared" si="25"/>
+      <c r="G221" s="28">
+        <f t="shared" si="35"/>
         <v>16.269999999999992</v>
       </c>
-      <c r="H217" s="28">
-        <f t="shared" si="25"/>
+      <c r="H221" s="28">
+        <f t="shared" si="35"/>
         <v>4.4367346938775505</v>
       </c>
-      <c r="I217" s="28">
-        <f t="shared" si="25"/>
+      <c r="I221" s="28">
+        <f t="shared" si="35"/>
         <v>11.897755102040817</v>
       </c>
-      <c r="J217" s="28">
-        <f t="shared" si="25"/>
+      <c r="J221" s="28">
+        <f t="shared" si="35"/>
         <v>40.88183673469387</v>
       </c>
-      <c r="K217" s="28">
-        <f t="shared" si="25"/>
+      <c r="K221" s="28">
+        <f t="shared" si="35"/>
         <v>67.627142857142843</v>
       </c>
-      <c r="L217" s="28">
-        <f t="shared" si="25"/>
+      <c r="L221" s="28">
+        <f t="shared" si="35"/>
         <v>0.58140816326530609</v>
       </c>
-      <c r="M217" s="28">
-        <f t="shared" si="25"/>
+      <c r="M221" s="28">
+        <f t="shared" si="35"/>
         <v>4.7795918367346951E-2</v>
       </c>
-      <c r="N217" s="28">
-        <f t="shared" si="25"/>
-        <v>19.280624999999997</v>
-      </c>
-      <c r="O217" s="28">
-        <f t="shared" si="25"/>
+      <c r="N221" s="28">
+        <f t="shared" si="35"/>
+        <v>44.213673469387736</v>
+      </c>
+      <c r="O221" s="28">
+        <f t="shared" si="35"/>
         <v>2.4553265306122443</v>
       </c>
     </row>
-    <row r="218" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A218" s="1">
+    <row r="222" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A222" s="1">
         <f>COUNTIF($A$24:$A$176, "*Commons-Math*Repaired")</f>
         <v>49</v>
       </c>
-      <c r="B218" s="1" t="s">
+      <c r="B222" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C218" s="28">
-        <f t="shared" ref="C218:O218" si="26">AVERAGEIF($A$24:$A$176, "*Commons-Math*_Repaired", B$24:B$176)</f>
+      <c r="C222" s="28">
+        <f t="shared" ref="C222:O222" si="36">AVERAGEIF($A$24:$A$176, "*Commons-Math*_Repaired", B$24:B$176)</f>
         <v>3.4955102040816328</v>
       </c>
-      <c r="D218" s="28">
-        <f t="shared" si="26"/>
+      <c r="D222" s="28">
+        <f t="shared" si="36"/>
         <v>78.292040816326548</v>
       </c>
-      <c r="E218" s="28">
-        <f t="shared" si="26"/>
+      <c r="E222" s="28">
+        <f t="shared" si="36"/>
         <v>24.755918367346936</v>
       </c>
-      <c r="F218" s="28">
-        <f t="shared" si="26"/>
+      <c r="F222" s="28">
+        <f t="shared" si="36"/>
         <v>7.4893877551020438</v>
       </c>
-      <c r="G218" s="28">
-        <f t="shared" si="26"/>
+      <c r="G222" s="28">
+        <f t="shared" si="36"/>
         <v>16.020204081632652</v>
       </c>
-      <c r="H218" s="28">
-        <f t="shared" si="26"/>
+      <c r="H222" s="28">
+        <f t="shared" si="36"/>
         <v>4.3863265306122452</v>
       </c>
-      <c r="I218" s="28">
-        <f t="shared" si="26"/>
+      <c r="I222" s="28">
+        <f t="shared" si="36"/>
         <v>11.875102040816325</v>
       </c>
-      <c r="J218" s="28">
-        <f t="shared" si="26"/>
+      <c r="J222" s="28">
+        <f t="shared" si="36"/>
         <v>40.774897959183662</v>
       </c>
-      <c r="K218" s="28">
-        <f t="shared" si="26"/>
+      <c r="K222" s="28">
+        <f t="shared" si="36"/>
         <v>67.33612244897958</v>
       </c>
-      <c r="L218" s="28">
-        <f t="shared" si="26"/>
+      <c r="L222" s="28">
+        <f t="shared" si="36"/>
         <v>0.58471428571428574</v>
       </c>
-      <c r="M218" s="28">
-        <f t="shared" si="26"/>
+      <c r="M222" s="28">
+        <f t="shared" si="36"/>
         <v>4.7795918367346951E-2</v>
       </c>
-      <c r="N218" s="28">
-        <f t="shared" si="26"/>
-        <v>19.346041666666665</v>
-      </c>
-      <c r="O218" s="28">
-        <f t="shared" si="26"/>
+      <c r="N222" s="28">
+        <f t="shared" si="36"/>
+        <v>44.277755102040793</v>
+      </c>
+      <c r="O222" s="28">
+        <f t="shared" si="36"/>
         <v>2.4587959183673465</v>
       </c>
     </row>
-    <row r="220" spans="1:32" ht="30.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B220" s="12" t="s">
+    <row r="224" spans="1:32" ht="30.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B224" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="C220" s="12" t="s">
+      <c r="C224" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="D220" s="12" t="s">
+      <c r="D224" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="E220" s="12" t="s">
+      <c r="E224" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="F220" s="12" t="s">
+      <c r="F224" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G220" s="12" t="s">
+      <c r="G224" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="H220" s="12" t="s">
+      <c r="H224" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I220" s="12" t="s">
+      <c r="I224" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="J220" s="12" t="s">
+      <c r="J224" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="K220" s="12" t="s">
+      <c r="K224" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="L220" s="12" t="s">
+      <c r="L224" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="M220" s="12" t="s">
+      <c r="M224" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="N220" s="12" t="s">
+      <c r="N224" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="O220" s="12" t="s">
+      <c r="O224" s="12" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="221" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A221" s="1">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A225" s="1">
         <f>COUNTIF($A$24:$A$176, "*Jackrabbit-Oak*Buggy")</f>
         <v>2</v>
       </c>
-      <c r="B221" s="1" t="s">
+      <c r="B225" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C221" s="28">
-        <f t="shared" ref="C221:O221" si="27">AVERAGEIF($A$24:$A$176, "*Jackrabbit-Oak*_Buggy", B$24:B$176)</f>
+      <c r="C225" s="28">
+        <f t="shared" ref="C225:O225" si="37">AVERAGEIF($A$24:$A$176, "*Jackrabbit-Oak*_Buggy", B$24:B$176)</f>
         <v>1.62</v>
       </c>
-      <c r="D221" s="28">
-        <f t="shared" si="27"/>
+      <c r="D225" s="28">
+        <f t="shared" si="37"/>
         <v>87.5</v>
       </c>
-      <c r="E221" s="28">
-        <f t="shared" si="27"/>
+      <c r="E225" s="28">
+        <f t="shared" si="37"/>
         <v>6.5</v>
       </c>
-      <c r="F221" s="28">
-        <f t="shared" si="27"/>
+      <c r="F225" s="28">
+        <f t="shared" si="37"/>
         <v>3.12</v>
       </c>
-      <c r="G221" s="28">
-        <f t="shared" si="27"/>
+      <c r="G225" s="28">
+        <f t="shared" si="37"/>
         <v>3.12</v>
       </c>
-      <c r="H221" s="28">
-        <f t="shared" si="27"/>
+      <c r="H225" s="28">
+        <f t="shared" si="37"/>
         <v>2.75</v>
       </c>
-      <c r="I221" s="28">
-        <f t="shared" si="27"/>
+      <c r="I225" s="28">
+        <f t="shared" si="37"/>
         <v>5.88</v>
       </c>
-      <c r="J221" s="28">
-        <f t="shared" si="27"/>
+      <c r="J225" s="28">
+        <f t="shared" si="37"/>
         <v>9.6199999999999992</v>
       </c>
-      <c r="K221" s="28">
-        <f t="shared" si="27"/>
+      <c r="K225" s="28">
+        <f t="shared" si="37"/>
         <v>22.33</v>
       </c>
-      <c r="L221" s="28">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="M221" s="28">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="N221" s="28">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="O221" s="28">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="222" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A222" s="1">
+      <c r="L225" s="28">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="M225" s="28">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="N225" s="28">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="O225" s="28">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A226" s="1">
         <f>COUNTIF($A$24:$A$176, "*Jackrabbit-Oak*Fixed")</f>
         <v>2</v>
       </c>
-      <c r="B222" s="1" t="s">
+      <c r="B226" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C222" s="28">
-        <f t="shared" ref="C222:O222" si="28">AVERAGEIF($A$24:$A$176, "*Jackrabbit-Oak*_Fixed", B$24:B$176)</f>
+      <c r="C226" s="28">
+        <f t="shared" ref="C226:O226" si="38">AVERAGEIF($A$24:$A$176, "*Jackrabbit-Oak*_Fixed", B$24:B$176)</f>
         <v>1.62</v>
       </c>
-      <c r="D222" s="28">
-        <f t="shared" si="28"/>
+      <c r="D226" s="28">
+        <f t="shared" si="38"/>
         <v>87</v>
       </c>
-      <c r="E222" s="28">
-        <f t="shared" si="28"/>
+      <c r="E226" s="28">
+        <f t="shared" si="38"/>
         <v>7.12</v>
       </c>
-      <c r="F222" s="28">
-        <f t="shared" si="28"/>
+      <c r="F226" s="28">
+        <f t="shared" si="38"/>
         <v>3.5</v>
       </c>
-      <c r="G222" s="28">
-        <f t="shared" si="28"/>
+      <c r="G226" s="28">
+        <f t="shared" si="38"/>
         <v>3.38</v>
       </c>
-      <c r="H222" s="28">
-        <f t="shared" si="28"/>
+      <c r="H226" s="28">
+        <f t="shared" si="38"/>
         <v>2.88</v>
       </c>
-      <c r="I222" s="28">
-        <f t="shared" si="28"/>
+      <c r="I226" s="28">
+        <f t="shared" si="38"/>
         <v>6.38</v>
       </c>
-      <c r="J222" s="28">
-        <f t="shared" si="28"/>
+      <c r="J226" s="28">
+        <f t="shared" si="38"/>
         <v>10.5</v>
       </c>
-      <c r="K222" s="28">
-        <f t="shared" si="28"/>
+      <c r="K226" s="28">
+        <f t="shared" si="38"/>
         <v>25.41</v>
       </c>
-      <c r="L222" s="28">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="M222" s="28">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="N222" s="28">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="O222" s="28">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="223" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A223" s="1">
+      <c r="L226" s="28">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="M226" s="28">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="N226" s="28">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="O226" s="28">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A227" s="1">
         <f>COUNTIF($A$24:$A$176, "*Jackrabbit-Oak*Repaired")</f>
         <v>2</v>
       </c>
-      <c r="B223" s="1" t="s">
+      <c r="B227" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C223" s="28">
-        <f t="shared" ref="C223:O223" si="29">AVERAGEIF($A$24:$A$176, "*Jackrabbit-Oak*_Repaired", B$24:B$176)</f>
+      <c r="C227" s="28">
+        <f t="shared" ref="C227:O227" si="39">AVERAGEIF($A$24:$A$176, "*Jackrabbit-Oak*_Repaired", B$24:B$176)</f>
         <v>1.6850000000000001</v>
       </c>
-      <c r="D223" s="28">
-        <f t="shared" si="29"/>
+      <c r="D227" s="28">
+        <f t="shared" si="39"/>
         <v>87.31</v>
       </c>
-      <c r="E223" s="28">
-        <f t="shared" si="29"/>
+      <c r="E227" s="28">
+        <f t="shared" si="39"/>
         <v>6.3100000000000005</v>
       </c>
-      <c r="F223" s="28">
-        <f t="shared" si="29"/>
+      <c r="F227" s="28">
+        <f t="shared" si="39"/>
         <v>3.25</v>
       </c>
-      <c r="G223" s="28">
-        <f t="shared" si="29"/>
+      <c r="G227" s="28">
+        <f t="shared" si="39"/>
         <v>3.25</v>
       </c>
-      <c r="H223" s="28">
-        <f t="shared" si="29"/>
+      <c r="H227" s="28">
+        <f t="shared" si="39"/>
         <v>2.75</v>
       </c>
-      <c r="I223" s="28">
-        <f t="shared" si="29"/>
+      <c r="I227" s="28">
+        <f t="shared" si="39"/>
         <v>6</v>
       </c>
-      <c r="J223" s="28">
-        <f t="shared" si="29"/>
+      <c r="J227" s="28">
+        <f t="shared" si="39"/>
         <v>9.5650000000000013</v>
       </c>
-      <c r="K223" s="28">
-        <f t="shared" si="29"/>
+      <c r="K227" s="28">
+        <f t="shared" si="39"/>
         <v>22.880000000000003</v>
       </c>
-      <c r="L223" s="28">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="M223" s="28">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="N223" s="28">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="O223" s="28">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A226" s="26" t="s">
+      <c r="L227" s="28">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="M227" s="28">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="N227" s="28">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="O227" s="28">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A230" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="B226" s="27"/>
-      <c r="C226" s="29"/>
-      <c r="D226" s="29"/>
-      <c r="E226" s="29"/>
-      <c r="F226" s="29"/>
-      <c r="G226" s="29"/>
-      <c r="H226" s="29"/>
-      <c r="I226" s="29"/>
-      <c r="J226" s="29"/>
-      <c r="K226" s="29"/>
-      <c r="L226" s="29"/>
-      <c r="M226" s="29"/>
-      <c r="N226" s="29"/>
-      <c r="O226" s="29"/>
-    </row>
-    <row r="227" spans="1:15" ht="15" x14ac:dyDescent="0.35">
-      <c r="A227"/>
-      <c r="B227"/>
-      <c r="C227"/>
-      <c r="D227"/>
-      <c r="E227"/>
-      <c r="F227"/>
-      <c r="G227"/>
-      <c r="H227"/>
-      <c r="I227"/>
-      <c r="J227"/>
-      <c r="K227"/>
-      <c r="L227"/>
-      <c r="M227"/>
-      <c r="N227"/>
-      <c r="O227"/>
-    </row>
-    <row r="228" spans="1:15" ht="28.8" x14ac:dyDescent="0.35">
-      <c r="A228" s="12" t="s">
+      <c r="B230" s="27"/>
+      <c r="C230" s="29"/>
+      <c r="D230" s="29"/>
+      <c r="E230" s="29"/>
+      <c r="F230" s="29"/>
+      <c r="G230" s="29"/>
+      <c r="H230" s="29"/>
+      <c r="I230" s="29"/>
+      <c r="J230" s="29"/>
+      <c r="K230" s="29"/>
+      <c r="L230" s="29"/>
+      <c r="M230" s="29"/>
+      <c r="N230" s="29"/>
+      <c r="O230" s="29"/>
+    </row>
+    <row r="231" spans="1:15" ht="15" x14ac:dyDescent="0.35">
+      <c r="A231"/>
+      <c r="B231"/>
+      <c r="C231"/>
+      <c r="D231"/>
+      <c r="E231"/>
+      <c r="F231"/>
+      <c r="G231"/>
+      <c r="H231"/>
+      <c r="I231"/>
+      <c r="J231"/>
+      <c r="K231"/>
+      <c r="L231"/>
+      <c r="M231"/>
+      <c r="N231"/>
+      <c r="O231"/>
+    </row>
+    <row r="232" spans="1:15" ht="28.8" x14ac:dyDescent="0.35">
+      <c r="A232" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="B228" s="12" t="s">
+      <c r="B232" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="C228" s="12" t="s">
+      <c r="C232" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="D228" s="12" t="s">
+      <c r="D232" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="E228" s="12" t="s">
+      <c r="E232" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="F228" s="12" t="s">
+      <c r="F232" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G228" s="12" t="s">
+      <c r="G232" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="H228" s="12" t="s">
+      <c r="H232" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I228" s="12" t="s">
+      <c r="I232" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="J228" s="12" t="s">
+      <c r="J232" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="K228" s="12" t="s">
+      <c r="K232" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="L228" s="12" t="s">
+      <c r="L232" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="M228" s="12" t="s">
+      <c r="M232" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="N228" s="12" t="s">
+      <c r="N232" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="O228" s="12" t="s">
+      <c r="O232" s="12" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A229" s="1">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A233" s="1">
         <f>COUNTIF($A$24:$A$176, "Arja*Fixed")</f>
         <v>21</v>
       </c>
-      <c r="B229" s="1" t="s">
+      <c r="B233" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C229" s="28">
-        <f t="shared" ref="C229:O229" si="30">AVERAGEIF($A$24:$A$176, "Arja*Fixed", B$24:B$176)</f>
+      <c r="C233" s="28">
+        <f t="shared" ref="C233:O233" si="40">AVERAGEIF($A$24:$A$176, "Arja*Fixed", B$24:B$176)</f>
         <v>3.9533333333333331</v>
       </c>
-      <c r="D229" s="28">
-        <f t="shared" si="30"/>
+      <c r="D233" s="28">
+        <f t="shared" si="40"/>
         <v>76.475238095238083</v>
       </c>
-      <c r="E229" s="28">
-        <f t="shared" si="30"/>
+      <c r="E233" s="28">
+        <f t="shared" si="40"/>
         <v>31.231428571428566</v>
       </c>
-      <c r="F229" s="28">
-        <f t="shared" si="30"/>
+      <c r="F233" s="28">
+        <f t="shared" si="40"/>
         <v>7.8638095238095236</v>
       </c>
-      <c r="G229" s="28">
-        <f t="shared" si="30"/>
+      <c r="G233" s="28">
+        <f t="shared" si="40"/>
         <v>19.423333333333332</v>
       </c>
-      <c r="H229" s="28">
-        <f t="shared" si="30"/>
+      <c r="H233" s="28">
+        <f t="shared" si="40"/>
         <v>4.6747619047619038</v>
       </c>
-      <c r="I229" s="28">
-        <f t="shared" si="30"/>
+      <c r="I233" s="28">
+        <f t="shared" si="40"/>
         <v>12.537619047619049</v>
       </c>
-      <c r="J229" s="28">
-        <f t="shared" si="30"/>
+      <c r="J233" s="28">
+        <f t="shared" si="40"/>
         <v>50.656190476190488</v>
       </c>
-      <c r="K229" s="28">
-        <f t="shared" si="30"/>
+      <c r="K233" s="28">
+        <f t="shared" si="40"/>
         <v>76.446190476190466</v>
       </c>
-      <c r="L229" s="28">
-        <f t="shared" si="30"/>
+      <c r="L233" s="28">
+        <f t="shared" si="40"/>
         <v>0.64428571428571413</v>
       </c>
-      <c r="M229" s="28">
-        <f t="shared" si="30"/>
+      <c r="M233" s="28">
+        <f t="shared" si="40"/>
         <v>4.5809523809523814E-2</v>
       </c>
-      <c r="N229" s="28">
-        <f t="shared" si="30"/>
+      <c r="N233" s="28">
+        <f t="shared" si="40"/>
         <v>19.481904761904762</v>
       </c>
-      <c r="O229" s="28">
-        <f t="shared" si="30"/>
+      <c r="O233" s="28">
+        <f t="shared" si="40"/>
         <v>1.0814285714285716</v>
       </c>
     </row>
-    <row r="230" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A230" s="30">
+    <row r="234" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A234" s="30">
         <f>COUNTIF($A$24:$A$176, "Arja*Repaired")</f>
         <v>21</v>
       </c>
-      <c r="B230" s="30" t="s">
+      <c r="B234" s="30" t="s">
         <v>219</v>
       </c>
-      <c r="C230" s="31">
-        <f t="shared" ref="C230:O230" si="31">AVERAGEIF($A$24:$A$176, "Arja*Repaired", B$24:B$176)</f>
+      <c r="C234" s="31">
+        <f t="shared" ref="C234:O234" si="41">AVERAGEIF($A$24:$A$176, "Arja*Repaired", B$24:B$176)</f>
         <v>4.0628571428571432</v>
       </c>
-      <c r="D230" s="31">
-        <f t="shared" si="31"/>
+      <c r="D234" s="31">
+        <f t="shared" si="41"/>
         <v>76.583333333333329</v>
       </c>
-      <c r="E230" s="31">
-        <f t="shared" si="31"/>
+      <c r="E234" s="31">
+        <f t="shared" si="41"/>
         <v>31.759999999999998</v>
       </c>
-      <c r="F230" s="31">
-        <f t="shared" si="31"/>
+      <c r="F234" s="31">
+        <f t="shared" si="41"/>
         <v>7.8466666666666667</v>
       </c>
-      <c r="G230" s="31">
-        <f t="shared" si="31"/>
+      <c r="G234" s="31">
+        <f t="shared" si="41"/>
         <v>19.358095238095238</v>
       </c>
-      <c r="H230" s="31">
-        <f t="shared" si="31"/>
+      <c r="H234" s="31">
+        <f t="shared" si="41"/>
         <v>4.6842857142857151</v>
       </c>
-      <c r="I230" s="31">
-        <f t="shared" si="31"/>
+      <c r="I234" s="31">
+        <f t="shared" si="41"/>
         <v>12.530000000000003</v>
       </c>
-      <c r="J230" s="31">
-        <f t="shared" si="31"/>
+      <c r="J234" s="31">
+        <f t="shared" si="41"/>
         <v>51.119047619047606</v>
       </c>
-      <c r="K230" s="31">
-        <f t="shared" si="31"/>
+      <c r="K234" s="31">
+        <f t="shared" si="41"/>
         <v>76.477142857142852</v>
       </c>
-      <c r="L230" s="31">
-        <f t="shared" si="31"/>
+      <c r="L234" s="31">
+        <f t="shared" si="41"/>
         <v>0.64428571428571413</v>
       </c>
-      <c r="M230" s="31">
-        <f t="shared" si="31"/>
+      <c r="M234" s="31">
+        <f t="shared" si="41"/>
         <v>4.5809523809523814E-2</v>
       </c>
-      <c r="N230" s="31">
-        <f t="shared" si="31"/>
+      <c r="N234" s="31">
+        <f t="shared" si="41"/>
         <v>19.481904761904762</v>
       </c>
-      <c r="O230" s="31">
-        <f t="shared" si="31"/>
+      <c r="O234" s="31">
+        <f t="shared" si="41"/>
         <v>1.0814285714285716</v>
       </c>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A231" s="1">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A235" s="1">
         <f>COUNTIF($A$24:$A$176, "GenProg*Fixed")</f>
         <v>13</v>
       </c>
-      <c r="B231" s="1" t="s">
+      <c r="B235" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C231" s="28">
-        <f t="shared" ref="C231:O231" si="32">AVERAGEIF($A$24:$A$176, "GenProg*Fixed", B$24:B$176)</f>
+      <c r="C235" s="28">
+        <f t="shared" ref="C235:O235" si="42">AVERAGEIF($A$24:$A$176, "GenProg*Fixed", B$24:B$176)</f>
         <v>2.9007692307692308</v>
       </c>
-      <c r="D231" s="28">
-        <f t="shared" si="32"/>
+      <c r="D235" s="28">
+        <f t="shared" si="42"/>
         <v>80.19923076923078</v>
       </c>
-      <c r="E231" s="28">
-        <f t="shared" si="32"/>
+      <c r="E235" s="28">
+        <f t="shared" si="42"/>
         <v>18.531538461538464</v>
       </c>
-      <c r="F231" s="28">
-        <f t="shared" si="32"/>
+      <c r="F235" s="28">
+        <f t="shared" si="42"/>
         <v>7.2492307692307696</v>
       </c>
-      <c r="G231" s="28">
-        <f t="shared" si="32"/>
+      <c r="G235" s="28">
+        <f t="shared" si="42"/>
         <v>13.443846153846156</v>
       </c>
-      <c r="H231" s="28">
-        <f t="shared" si="32"/>
+      <c r="H235" s="28">
+        <f t="shared" si="42"/>
         <v>4.37</v>
       </c>
-      <c r="I231" s="28">
-        <f t="shared" si="32"/>
+      <c r="I235" s="28">
+        <f t="shared" si="42"/>
         <v>11.61923076923077</v>
       </c>
-      <c r="J231" s="28">
-        <f t="shared" si="32"/>
+      <c r="J235" s="28">
+        <f t="shared" si="42"/>
         <v>31.976153846153842</v>
       </c>
-      <c r="K231" s="28">
-        <f t="shared" si="32"/>
+      <c r="K235" s="28">
+        <f t="shared" si="42"/>
         <v>60.873076923076937</v>
       </c>
-      <c r="L231" s="28">
-        <f t="shared" si="32"/>
+      <c r="L235" s="28">
+        <f t="shared" si="42"/>
         <v>0.57000000000000006</v>
       </c>
-      <c r="M231" s="28">
-        <f t="shared" si="32"/>
+      <c r="M235" s="28">
+        <f t="shared" si="42"/>
         <v>3.6615384615384619E-2</v>
       </c>
-      <c r="N231" s="28">
-        <f t="shared" si="32"/>
-        <v>19.249166666666667</v>
-      </c>
-      <c r="O231" s="28">
-        <f t="shared" si="32"/>
+      <c r="N235" s="28">
+        <f t="shared" si="42"/>
+        <v>113.23</v>
+      </c>
+      <c r="O235" s="28">
+        <f t="shared" si="42"/>
         <v>6.2876923076923088</v>
       </c>
     </row>
-    <row r="232" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A232" s="30">
+    <row r="236" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A236" s="30">
         <f>COUNTIF($A$24:$A$176, "GenProg*Repaired")</f>
         <v>13</v>
       </c>
-      <c r="B232" s="30" t="s">
+      <c r="B236" s="30" t="s">
         <v>221</v>
       </c>
-      <c r="C232" s="31">
-        <f t="shared" ref="C232:O232" si="33">AVERAGEIF($A$24:$A$176, "GenProg*Repaired", B$24:B$176)</f>
+      <c r="C236" s="31">
+        <f t="shared" ref="C236:O236" si="43">AVERAGEIF($A$24:$A$176, "GenProg*Repaired", B$24:B$176)</f>
         <v>2.7846153846153849</v>
       </c>
-      <c r="D232" s="31">
-        <f t="shared" si="33"/>
+      <c r="D236" s="31">
+        <f t="shared" si="43"/>
         <v>80.377692307692314</v>
       </c>
-      <c r="E232" s="31">
-        <f t="shared" si="33"/>
+      <c r="E236" s="31">
+        <f t="shared" si="43"/>
         <v>18.165384615384617</v>
       </c>
-      <c r="F232" s="31">
-        <f t="shared" si="33"/>
+      <c r="F236" s="31">
+        <f t="shared" si="43"/>
         <v>7.3276923076923062</v>
       </c>
-      <c r="G232" s="31">
-        <f t="shared" si="33"/>
+      <c r="G236" s="31">
+        <f t="shared" si="43"/>
         <v>12.911538461538461</v>
       </c>
-      <c r="H232" s="31">
-        <f t="shared" si="33"/>
+      <c r="H236" s="31">
+        <f t="shared" si="43"/>
         <v>4.24</v>
       </c>
-      <c r="I232" s="31">
-        <f t="shared" si="33"/>
+      <c r="I236" s="31">
+        <f t="shared" si="43"/>
         <v>11.56769230769231</v>
       </c>
-      <c r="J232" s="31">
-        <f t="shared" si="33"/>
+      <c r="J236" s="31">
+        <f t="shared" si="43"/>
         <v>31.073076923076922</v>
       </c>
-      <c r="K232" s="31">
-        <f t="shared" si="33"/>
+      <c r="K236" s="31">
+        <f t="shared" si="43"/>
         <v>60.154615384615404</v>
       </c>
-      <c r="L232" s="31">
-        <f t="shared" si="33"/>
+      <c r="L236" s="31">
+        <f t="shared" si="43"/>
         <v>0.57000000000000006</v>
       </c>
-      <c r="M232" s="31">
-        <f t="shared" si="33"/>
+      <c r="M236" s="31">
+        <f t="shared" si="43"/>
         <v>3.6615384615384619E-2</v>
       </c>
-      <c r="N232" s="31">
-        <f t="shared" si="33"/>
-        <v>19.249166666666667</v>
-      </c>
-      <c r="O232" s="31">
-        <f t="shared" si="33"/>
+      <c r="N236" s="31">
+        <f t="shared" si="43"/>
+        <v>113.23</v>
+      </c>
+      <c r="O236" s="31">
+        <f t="shared" si="43"/>
         <v>6.2876923076923088</v>
       </c>
     </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A233" s="1">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A237" s="1">
         <f>COUNTIF($A$24:$A$176, "Kali*Fixed")</f>
         <v>3</v>
       </c>
-      <c r="B233" s="1" t="s">
+      <c r="B237" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C233" s="28">
-        <f t="shared" ref="C233:O233" si="34">AVERAGEIF($A$24:$A$176, "Kali*Fixed", B$24:B$176)</f>
+      <c r="C237" s="28">
+        <f t="shared" ref="C237:O237" si="44">AVERAGEIF($A$24:$A$176, "Kali*Fixed", B$24:B$176)</f>
         <v>2.0333333333333337</v>
       </c>
-      <c r="D233" s="28">
-        <f t="shared" si="34"/>
+      <c r="D237" s="28">
+        <f t="shared" si="44"/>
         <v>84.95</v>
       </c>
-      <c r="E233" s="28">
-        <f t="shared" si="34"/>
+      <c r="E237" s="28">
+        <f t="shared" si="44"/>
         <v>8.9666666666666668</v>
       </c>
-      <c r="F233" s="28">
-        <f t="shared" si="34"/>
+      <c r="F237" s="28">
+        <f t="shared" si="44"/>
         <v>4.7566666666666668</v>
       </c>
-      <c r="G233" s="28">
-        <f t="shared" si="34"/>
+      <c r="G237" s="28">
+        <f t="shared" si="44"/>
         <v>6.22</v>
       </c>
-      <c r="H233" s="28">
-        <f t="shared" si="34"/>
+      <c r="H237" s="28">
+        <f t="shared" si="44"/>
         <v>2.8933333333333331</v>
       </c>
-      <c r="I233" s="28">
-        <f t="shared" si="34"/>
+      <c r="I237" s="28">
+        <f t="shared" si="44"/>
         <v>7.6499999999999995</v>
       </c>
-      <c r="J233" s="28">
-        <f t="shared" si="34"/>
+      <c r="J237" s="28">
+        <f t="shared" si="44"/>
         <v>15.186666666666667</v>
       </c>
-      <c r="K233" s="28">
-        <f t="shared" si="34"/>
+      <c r="K237" s="28">
+        <f t="shared" si="44"/>
         <v>33.646666666666668</v>
       </c>
-      <c r="L233" s="28">
-        <f t="shared" si="34"/>
+      <c r="L237" s="28">
+        <f t="shared" si="44"/>
         <v>0.78333333333333333</v>
       </c>
-      <c r="M233" s="28">
-        <f t="shared" si="34"/>
+      <c r="M237" s="28">
+        <f t="shared" si="44"/>
         <v>4.2666666666666665E-2</v>
       </c>
-      <c r="N233" s="28">
-        <f t="shared" si="34"/>
+      <c r="N237" s="28">
+        <f t="shared" si="44"/>
         <v>32.659999999999997</v>
       </c>
-      <c r="O233" s="28">
-        <f t="shared" si="34"/>
+      <c r="O237" s="28">
+        <f t="shared" si="44"/>
         <v>1.8133333333333335</v>
       </c>
     </row>
-    <row r="234" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A234" s="30">
+    <row r="238" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A238" s="30">
         <f>COUNTIF($A$24:$A$176, "Kali*Repaired")</f>
         <v>3</v>
       </c>
-      <c r="B234" s="30" t="s">
+      <c r="B238" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="C234" s="31">
-        <f t="shared" ref="C234:O234" si="35">AVERAGEIF($A$24:$A$176, "Kali*Repaired", B$24:B$176)</f>
+      <c r="C238" s="31">
+        <f t="shared" ref="C238:O238" si="45">AVERAGEIF($A$24:$A$176, "Kali*Repaired", B$24:B$176)</f>
         <v>2.0066666666666664</v>
       </c>
-      <c r="D234" s="31">
-        <f t="shared" si="35"/>
+      <c r="D238" s="31">
+        <f t="shared" si="45"/>
         <v>85.096666666666678</v>
       </c>
-      <c r="E234" s="31">
-        <f t="shared" si="35"/>
+      <c r="E238" s="31">
+        <f t="shared" si="45"/>
         <v>8.4600000000000009</v>
       </c>
-      <c r="F234" s="31">
-        <f t="shared" si="35"/>
+      <c r="F238" s="31">
+        <f t="shared" si="45"/>
         <v>4.7433333333333332</v>
       </c>
-      <c r="G234" s="31">
-        <f t="shared" si="35"/>
+      <c r="G238" s="31">
+        <f t="shared" si="45"/>
         <v>5.9233333333333329</v>
       </c>
-      <c r="H234" s="31">
-        <f t="shared" si="35"/>
+      <c r="H238" s="31">
+        <f t="shared" si="45"/>
         <v>2.7766666666666668</v>
       </c>
-      <c r="I234" s="31">
-        <f t="shared" si="35"/>
+      <c r="I238" s="31">
+        <f t="shared" si="45"/>
         <v>7.5166666666666666</v>
       </c>
-      <c r="J234" s="31">
-        <f t="shared" si="35"/>
+      <c r="J238" s="31">
+        <f t="shared" si="45"/>
         <v>14.383333333333335</v>
       </c>
-      <c r="K234" s="31">
-        <f t="shared" si="35"/>
+      <c r="K238" s="31">
+        <f t="shared" si="45"/>
         <v>32.49</v>
       </c>
-      <c r="L234" s="31">
-        <f t="shared" si="35"/>
+      <c r="L238" s="31">
+        <f t="shared" si="45"/>
         <v>0.78333333333333333</v>
       </c>
-      <c r="M234" s="31">
-        <f t="shared" si="35"/>
+      <c r="M238" s="31">
+        <f t="shared" si="45"/>
         <v>4.2666666666666665E-2</v>
       </c>
-      <c r="N234" s="31">
-        <f t="shared" si="35"/>
+      <c r="N238" s="31">
+        <f t="shared" si="45"/>
         <v>32.659999999999997</v>
       </c>
-      <c r="O234" s="31">
-        <f t="shared" si="35"/>
+      <c r="O238" s="31">
+        <f t="shared" si="45"/>
         <v>1.8133333333333335</v>
       </c>
     </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A235" s="1">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A239" s="1">
         <f>COUNTIF($A$24:$A$176, "Nopol*Fixed")</f>
         <v>1</v>
       </c>
-      <c r="B235" s="1" t="s">
+      <c r="B239" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C235" s="28">
-        <f t="shared" ref="C235:O235" si="36">AVERAGEIF($A$24:$A$176, "Nopol*Fixed", B$24:B$176)</f>
+      <c r="C239" s="28">
+        <f t="shared" ref="C239:O239" si="46">AVERAGEIF($A$24:$A$176, "Nopol*Fixed", B$24:B$176)</f>
         <v>3.29</v>
       </c>
-      <c r="D235" s="28">
-        <f t="shared" si="36"/>
+      <c r="D239" s="28">
+        <f t="shared" si="46"/>
         <v>75.73</v>
       </c>
-      <c r="E235" s="28">
-        <f t="shared" si="36"/>
+      <c r="E239" s="28">
+        <f t="shared" si="46"/>
         <v>20.88</v>
       </c>
-      <c r="F235" s="28">
-        <f t="shared" si="36"/>
+      <c r="F239" s="28">
+        <f t="shared" si="46"/>
         <v>8.51</v>
       </c>
-      <c r="G235" s="28">
-        <f t="shared" si="36"/>
+      <c r="G239" s="28">
+        <f t="shared" si="46"/>
         <v>16.670000000000002</v>
       </c>
-      <c r="H235" s="28">
-        <f t="shared" si="36"/>
+      <c r="H239" s="28">
+        <f t="shared" si="46"/>
         <v>5.0199999999999996</v>
       </c>
-      <c r="I235" s="28">
-        <f t="shared" si="36"/>
+      <c r="I239" s="28">
+        <f t="shared" si="46"/>
         <v>13.53</v>
       </c>
-      <c r="J235" s="28">
-        <f t="shared" si="36"/>
+      <c r="J239" s="28">
+        <f t="shared" si="46"/>
         <v>37.549999999999997</v>
       </c>
-      <c r="K235" s="28">
-        <f t="shared" si="36"/>
+      <c r="K239" s="28">
+        <f t="shared" si="46"/>
         <v>73.849999999999994</v>
       </c>
-      <c r="L235" s="28">
-        <f t="shared" si="36"/>
+      <c r="L239" s="28">
+        <f t="shared" si="46"/>
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="M235" s="28">
-        <f t="shared" si="36"/>
+      <c r="M239" s="28">
+        <f t="shared" si="46"/>
         <v>3.9E-2</v>
       </c>
-      <c r="N235" s="28">
-        <f t="shared" si="36"/>
+      <c r="N239" s="28">
+        <f t="shared" si="46"/>
         <v>2.4300000000000002</v>
       </c>
-      <c r="O235" s="28">
-        <f t="shared" si="36"/>
+      <c r="O239" s="28">
+        <f t="shared" si="46"/>
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="236" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A236" s="30">
+    <row r="240" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A240" s="30">
         <f>COUNTIF($A$24:$A$176, "Nopol*Repaired")</f>
         <v>1</v>
       </c>
-      <c r="B236" s="30" t="s">
+      <c r="B240" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="C236" s="31">
-        <f t="shared" ref="C236:O236" si="37">AVERAGEIF($A$24:$A$176, "Nopol*Repaired", B$24:B$176)</f>
+      <c r="C240" s="31">
+        <f t="shared" ref="C240:O240" si="47">AVERAGEIF($A$24:$A$176, "Nopol*Repaired", B$24:B$176)</f>
         <v>3.59</v>
       </c>
-      <c r="D236" s="31">
-        <f t="shared" si="37"/>
+      <c r="D240" s="31">
+        <f t="shared" si="47"/>
         <v>75.3</v>
       </c>
-      <c r="E236" s="31">
-        <f t="shared" si="37"/>
+      <c r="E240" s="31">
+        <f t="shared" si="47"/>
         <v>21.44</v>
       </c>
-      <c r="F236" s="31">
-        <f t="shared" si="37"/>
+      <c r="F240" s="31">
+        <f t="shared" si="47"/>
         <v>8.61</v>
       </c>
-      <c r="G236" s="31">
-        <f t="shared" si="37"/>
+      <c r="G240" s="31">
+        <f t="shared" si="47"/>
         <v>17.2</v>
       </c>
-      <c r="H236" s="31">
-        <f t="shared" si="37"/>
+      <c r="H240" s="31">
+        <f t="shared" si="47"/>
         <v>5.31</v>
       </c>
-      <c r="I236" s="31">
-        <f t="shared" si="37"/>
+      <c r="I240" s="31">
+        <f t="shared" si="47"/>
         <v>13.93</v>
       </c>
-      <c r="J236" s="31">
-        <f t="shared" si="37"/>
+      <c r="J240" s="31">
+        <f t="shared" si="47"/>
         <v>38.65</v>
       </c>
-      <c r="K236" s="31">
-        <f t="shared" si="37"/>
+      <c r="K240" s="31">
+        <f t="shared" si="47"/>
         <v>76.17</v>
       </c>
-      <c r="L236" s="31">
-        <f t="shared" si="37"/>
+      <c r="L240" s="31">
+        <f t="shared" si="47"/>
         <v>0.26</v>
       </c>
-      <c r="M236" s="31">
-        <f t="shared" si="37"/>
+      <c r="M240" s="31">
+        <f t="shared" si="47"/>
         <v>3.9E-2</v>
       </c>
-      <c r="N236" s="31">
-        <f t="shared" si="37"/>
+      <c r="N240" s="31">
+        <f t="shared" si="47"/>
         <v>5.57</v>
       </c>
-      <c r="O236" s="31">
-        <f t="shared" si="37"/>
+      <c r="O240" s="31">
+        <f t="shared" si="47"/>
         <v>0.31</v>
       </c>
     </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A237" s="1">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A241" s="1">
         <f>COUNTIF($A$24:$A$176, "RSRepair*Fixed")</f>
         <v>8</v>
       </c>
-      <c r="B237" s="1" t="s">
+      <c r="B241" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C237" s="28">
-        <f t="shared" ref="C237:O237" si="38">AVERAGEIF($A$24:$A$176, "RSRepair*Fixed", B$24:B$176)</f>
+      <c r="C241" s="28">
+        <f t="shared" ref="C241:O241" si="48">AVERAGEIF($A$24:$A$176, "RSRepair*Fixed", B$24:B$176)</f>
         <v>3.6725000000000003</v>
       </c>
-      <c r="D237" s="28">
-        <f t="shared" si="38"/>
+      <c r="D241" s="28">
+        <f t="shared" si="48"/>
         <v>76.286249999999995</v>
       </c>
-      <c r="E237" s="28">
-        <f t="shared" si="38"/>
+      <c r="E241" s="28">
+        <f t="shared" si="48"/>
         <v>27.195</v>
       </c>
-      <c r="F237" s="28">
-        <f t="shared" si="38"/>
+      <c r="F241" s="28">
+        <f t="shared" si="48"/>
         <v>8.1512499999999992</v>
       </c>
-      <c r="G237" s="28">
-        <f t="shared" si="38"/>
+      <c r="G241" s="28">
+        <f t="shared" si="48"/>
         <v>17.8</v>
       </c>
-      <c r="H237" s="28">
-        <f t="shared" si="38"/>
+      <c r="H241" s="28">
+        <f t="shared" si="48"/>
         <v>4.6725000000000003</v>
       </c>
-      <c r="I237" s="28">
-        <f t="shared" si="38"/>
+      <c r="I241" s="28">
+        <f t="shared" si="48"/>
         <v>12.823750000000002</v>
       </c>
-      <c r="J237" s="28">
-        <f t="shared" si="38"/>
+      <c r="J241" s="28">
+        <f t="shared" si="48"/>
         <v>44.994999999999997</v>
       </c>
-      <c r="K237" s="28">
-        <f t="shared" si="38"/>
+      <c r="K241" s="28">
+        <f t="shared" si="48"/>
         <v>74.61375000000001</v>
       </c>
-      <c r="L237" s="28">
-        <f t="shared" si="38"/>
+      <c r="L241" s="28">
+        <f t="shared" si="48"/>
         <v>0.48875000000000002</v>
       </c>
-      <c r="M237" s="28">
-        <f t="shared" si="38"/>
+      <c r="M241" s="28">
+        <f t="shared" si="48"/>
         <v>3.5500000000000004E-2</v>
       </c>
-      <c r="N237" s="28">
-        <f t="shared" si="38"/>
+      <c r="N241" s="28">
+        <f t="shared" si="48"/>
         <v>19.6175</v>
       </c>
-      <c r="O237" s="28">
-        <f t="shared" si="38"/>
+      <c r="O241" s="28">
+        <f t="shared" si="48"/>
         <v>1.0899999999999999</v>
       </c>
     </row>
-    <row r="238" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A238" s="30">
+    <row r="242" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A242" s="30">
         <f>COUNTIF($A$24:$A$176, "RSRepair*Repaired")</f>
         <v>8</v>
       </c>
-      <c r="B238" s="30" t="s">
+      <c r="B242" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="C238" s="31">
-        <f t="shared" ref="C238:O238" si="39">AVERAGEIF($A$24:$A$176, "RSRepair*Repaired", B$24:B$176)</f>
+      <c r="C242" s="31">
+        <f t="shared" ref="C242:O242" si="49">AVERAGEIF($A$24:$A$176, "RSRepair*Repaired", B$24:B$176)</f>
         <v>3.5812500000000003</v>
       </c>
-      <c r="D238" s="31">
-        <f t="shared" si="39"/>
+      <c r="D242" s="31">
+        <f t="shared" si="49"/>
         <v>76.556249999999991</v>
       </c>
-      <c r="E238" s="31">
-        <f t="shared" si="39"/>
+      <c r="E242" s="31">
+        <f t="shared" si="49"/>
         <v>26.94875</v>
       </c>
-      <c r="F238" s="31">
-        <f t="shared" si="39"/>
+      <c r="F242" s="31">
+        <f t="shared" si="49"/>
         <v>8.1187499999999986</v>
       </c>
-      <c r="G238" s="31">
-        <f t="shared" si="39"/>
+      <c r="G242" s="31">
+        <f t="shared" si="49"/>
         <v>17.056249999999999</v>
       </c>
-      <c r="H238" s="31">
-        <f t="shared" si="39"/>
+      <c r="H242" s="31">
+        <f t="shared" si="49"/>
         <v>4.5374999999999996</v>
       </c>
-      <c r="I238" s="31">
-        <f t="shared" si="39"/>
+      <c r="I242" s="31">
+        <f t="shared" si="49"/>
         <v>12.65625</v>
       </c>
-      <c r="J238" s="31">
-        <f t="shared" si="39"/>
+      <c r="J242" s="31">
+        <f t="shared" si="49"/>
         <v>44.002499999999998</v>
       </c>
-      <c r="K238" s="31">
-        <f t="shared" si="39"/>
+      <c r="K242" s="31">
+        <f t="shared" si="49"/>
         <v>73.032500000000013</v>
       </c>
-      <c r="L238" s="31">
-        <f t="shared" si="39"/>
+      <c r="L242" s="31">
+        <f t="shared" si="49"/>
         <v>0.48875000000000002</v>
       </c>
-      <c r="M238" s="31">
-        <f t="shared" si="39"/>
+      <c r="M242" s="31">
+        <f t="shared" si="49"/>
         <v>3.5500000000000004E-2</v>
       </c>
-      <c r="N238" s="31">
-        <f t="shared" si="39"/>
+      <c r="N242" s="31">
+        <f t="shared" si="49"/>
         <v>19.6175</v>
       </c>
-      <c r="O238" s="31">
-        <f t="shared" si="39"/>
+      <c r="O242" s="31">
+        <f t="shared" si="49"/>
         <v>1.0899999999999999</v>
       </c>
     </row>
@@ -16794,7 +16798,7 @@
       <formula>$P$75</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C217:O217 C222:O222 C190:O190 C197:O197 C201:O201 C205:O205 C209:O209 T197:AF197 T201:AF201 T205:AF205 T209:AF209 T213:AF213 C229:O229 C231:O231 C233:O233 C235:O235 C237:O237">
+  <conditionalFormatting sqref="C221:O221 C226:O226 C190:O190 C197:O197 C201:O201 C205:O205 C209:O209 T197:AF197 T201:AF201 T205:AF205 T209:AF209 C213:O213 C233:O233 C235:O235 C237:O237 C239:O239 C241:O241">
     <cfRule type="cellIs" dxfId="3" priority="53" operator="greaterThan">
       <formula>C191</formula>
     </cfRule>
@@ -16802,7 +16806,7 @@
       <formula>C191</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C218:O218 C223:O223 C191:O191 C198:O198 C202:O202 C206:O206 C210:O210 T198:AF198 T202:AF202 T206:AF206 T210:AF210 T214:AF214 C230:O230 C232:O232 C234:O234 C236:O236 C238:O238">
+  <conditionalFormatting sqref="C222:O222 C227:O227 C191:O191 C198:O198 C202:O202 C206:O206 C210:O210 T198:AF198 T202:AF202 T206:AF206 T210:AF210 C214:O214 C234:O234 C236:O236 C238:O238 C240:O240 C242:O242">
     <cfRule type="cellIs" dxfId="1" priority="54" operator="greaterThan">
       <formula>C190</formula>
     </cfRule>

</xml_diff>